<commit_message>
reverting back to original
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/ActivityData.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/ActivityData.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B42927D-5AAB-4DE1-98D1-40748D785E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737FA6E6-9307-4593-B5A6-D1E0CD531E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstrumentAttribute" sheetId="1" r:id="rId1"/>
-    <sheet name="xxTransactionActivity" sheetId="12" r:id="rId2"/>
-    <sheet name="TransactionActivity" sheetId="13" r:id="rId3"/>
+    <sheet name="TransactionActivity" sheetId="12" r:id="rId2"/>
+    <sheet name="xxTransactionActivity" sheetId="13" r:id="rId3"/>
     <sheet name="GLRule" sheetId="7" state="hidden" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="8" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TransactionActivity!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">xxTransactionActivity!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -404,16 +404,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1233,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0A9CC0-A1B0-44B9-AC56-19A480FED1A4}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,7 +2347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467D12F6-B29D-4EC9-9609-B26D1F8248BC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Checking in Whole population
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/ActivityData.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/ActivityData.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B351B1C-C9FF-42C2-8C2D-70F4F39F53D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9590231-1EDD-4E06-9CA3-C819F82A6401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12645" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstrumentAttribute" sheetId="1" r:id="rId1"/>
-    <sheet name="xxxTransactionActivity" sheetId="12" r:id="rId2"/>
-    <sheet name="TransactionActivity" sheetId="13" r:id="rId3"/>
+    <sheet name="TransactionActivity" sheetId="12" r:id="rId2"/>
+    <sheet name="xxTransactionActivity" sheetId="13" r:id="rId3"/>
     <sheet name="GLRule" sheetId="7" state="hidden" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="8" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TransactionActivity!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">xxTransactionActivity!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0A9CC0-A1B0-44B9-AC56-19A480FED1A4}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467D12F6-B29D-4EC9-9609-B26D1F8248BC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>